<commit_message>
Update met betrekking tot TaT in uiteindelijke schema
</commit_message>
<xml_diff>
--- a/FleetType.xlsx
+++ b/FleetType.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjribeiro/Documents/courses/AE4423 Airline Planning &amp; Optimisation/2025/Assignment2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllFiles\AE4423-20\AirlinePlanningOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{549D49D8-1F80-8E4A-A1FA-62F8DBF69681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2216A6F9-EDBD-4FD1-9390-2143FCB06DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{1484A53A-3F39-2A41-8004-4729A23DDD1B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1484A53A-3F39-2A41-8004-4729A23DDD1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Fleet Type" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -415,21 +418,21 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -445,7 +448,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -459,7 +462,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -473,7 +476,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -487,7 +490,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -501,7 +504,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -515,7 +518,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -529,7 +532,7 @@
         <v>11428.571428571429</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -543,7 +546,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -557,7 +560,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -571,7 +574,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>